<commit_message>
update: new raw data
</commit_message>
<xml_diff>
--- a/phmsa-clean/data/raw/lng2011toPresent.xlsx
+++ b/phmsa-clean/data/raw/lng2011toPresent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Pipeline Metrics Reporting\Ongoing Tasks and Work Instructions\Web Update\5-Significant Incident Data Files\SaveExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FEB2931-B90A-4E8A-9C0E-B2711FFC7066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{087D202F-678A-4C6F-89C8-5BA22A409D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{D8487664-C840-4563-B0DE-ADA9AB096849}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{3E2CFA4F-F756-41EC-880A-84AFD7F8E076}"/>
   </bookViews>
   <sheets>
     <sheet name="lng2011toPresentFields" sheetId="2" r:id="rId1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3579,7 +3580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96B33CF-0C73-42B4-883D-0C801F1AF3F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEE5712-522A-4B59-B7CB-30FADB34326A}">
   <sheetPr codeName="Sheet33"/>
   <dimension ref="A1:D224"/>
   <sheetViews>
@@ -6736,7 +6737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D068D962-71EE-4969-A0C3-FBB98EE3197A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714D9FBB-CA80-4578-9D52-1DA6E566E805}">
   <dimension ref="A1:HN33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -7466,7 +7467,7 @@
     </row>
     <row r="2" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>462</v>
@@ -7747,7 +7748,7 @@
     </row>
     <row r="3" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>462</v>
@@ -8007,7 +8008,7 @@
     </row>
     <row r="4" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>469</v>
@@ -8294,7 +8295,7 @@
     </row>
     <row r="5" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>462</v>
@@ -8572,7 +8573,7 @@
     </row>
     <row r="6" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>469</v>
@@ -8841,7 +8842,7 @@
     </row>
     <row r="7" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>462</v>
@@ -9113,7 +9114,7 @@
     </row>
     <row r="8" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>462</v>
@@ -9370,7 +9371,7 @@
     </row>
     <row r="9" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>462</v>
@@ -9642,7 +9643,7 @@
     </row>
     <row r="10" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>462</v>
@@ -9908,7 +9909,7 @@
     </row>
     <row r="11" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>469</v>
@@ -10168,7 +10169,7 @@
     </row>
     <row r="12" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>469</v>
@@ -10446,7 +10447,7 @@
     </row>
     <row r="13" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>462</v>
@@ -10721,7 +10722,7 @@
     </row>
     <row r="14" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>469</v>
@@ -11002,7 +11003,7 @@
     </row>
     <row r="15" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>462</v>
@@ -11265,7 +11266,7 @@
     </row>
     <row r="16" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>462</v>
@@ -11534,7 +11535,7 @@
     </row>
     <row r="17" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>462</v>
@@ -11806,7 +11807,7 @@
     </row>
     <row r="18" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>462</v>
@@ -12072,7 +12073,7 @@
     </row>
     <row r="19" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>469</v>
@@ -12341,7 +12342,7 @@
     </row>
     <row r="20" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>469</v>
@@ -12616,7 +12617,7 @@
     </row>
     <row r="21" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>462</v>
@@ -12882,7 +12883,7 @@
     </row>
     <row r="22" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>469</v>
@@ -13151,7 +13152,7 @@
     </row>
     <row r="23" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>469</v>
@@ -13447,7 +13448,7 @@
     </row>
     <row r="24" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>462</v>
@@ -13743,7 +13744,7 @@
     </row>
     <row r="25" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>462</v>
@@ -14027,7 +14028,7 @@
     </row>
     <row r="26" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>469</v>
@@ -14299,7 +14300,7 @@
     </row>
     <row r="27" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>462</v>
@@ -14586,7 +14587,7 @@
     </row>
     <row r="28" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>462</v>
@@ -14598,13 +14599,13 @@
         <v>20210005</v>
       </c>
       <c r="E28" s="12">
-        <v>36621</v>
+        <v>36641</v>
       </c>
       <c r="F28" s="14">
         <v>44477.429328703707</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>934</v>
+        <v>463</v>
       </c>
       <c r="H28" s="12">
         <v>15359</v>
@@ -14853,7 +14854,7 @@
         <v>962</v>
       </c>
       <c r="HI28" s="14">
-        <v>44679</v>
+        <v>44685</v>
       </c>
       <c r="HJ28" s="12" t="s">
         <v>958</v>
@@ -14873,7 +14874,7 @@
     </row>
     <row r="29" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>462</v>
@@ -15154,7 +15155,7 @@
     </row>
     <row r="30" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>462</v>
@@ -15444,7 +15445,7 @@
     </row>
     <row r="31" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>462</v>
@@ -15722,7 +15723,7 @@
     </row>
     <row r="32" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>462</v>
@@ -16021,7 +16022,7 @@
     </row>
     <row r="33" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="14">
-        <v>44680.416817129626</v>
+        <v>44712.391365740739</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>462</v>
@@ -16299,5 +16300,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: new raw incident data
</commit_message>
<xml_diff>
--- a/phmsa-clean/data/raw/lng2011toPresent.xlsx
+++ b/phmsa-clean/data/raw/lng2011toPresent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Pipeline Metrics Reporting\Ongoing Tasks and Work Instructions\Web Update\5-Significant Incident Data Files\SaveExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{087D202F-678A-4C6F-89C8-5BA22A409D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{938E2436-DF72-4BF6-BA96-96F6BA2DB00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{3E2CFA4F-F756-41EC-880A-84AFD7F8E076}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{71B5579A-CF57-4DE7-8784-5549CE4C9B70}"/>
   </bookViews>
   <sheets>
     <sheet name="lng2011toPresentFields" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="1036">
   <si>
     <t>Liquefied Natural Gas (LNG) Facilities Incidents for 2011 - present (PHMSA Form 7100.3 Rev. 9-2019) - Data Dictionary for Flagged Data file</t>
   </si>
@@ -3095,9 +3095,6 @@
   </si>
   <si>
     <t>AN UNINTENTIONAL DISCHARGE OF NATURAL GAS OCCURRED DURING NITROGEN DISPLACEMENT ACTIVITIES ASSOCIATED WITH COMMISSIONING OF THE SOUTH LNG TANK.  NITROGEN MUST BE REMOVED FROM THE TANK, PRIOR TO THE INITIAL START-UP, BY FLOWING NATURAL GAS INTO THE TANK IN ORDER TO DISPLACE THE NITROGEN.    THE FACILITY AND ITS PRIMARY CONTRACTOR DEVELOPED A PROCEDURE FOR CARRYING OUT THE NITROGEN DISPLACEMENT ACTIVITIES THAT INITIALLY INCLUDED DIRECTING THE VENT STREAM TO THE LP FLARE. LATER, THE PROCEDURE WAS AMENDED TO PROVIDE FOR VENTING OF THE NITROGEN VIA A ROOF VENT ON THE LNG TANK.  THE FACILITY COMPLETED A MANAGEMENT OF CHANGE ("MOC") EVALUATION FOR THE AMENDED PROCEDURE, WHICH WAS APPROVED BY OPERATIONS, COMMISSIONING, AND ENGINEERING.  ACCORDING TO THE AMENDED PROCEDURE, THE VENTING WOULD BE MONITORED TO DETERMINE WHEN THE NITROGEN DISPLACEMENT WOULD BE COMPLETE AND THE REMAINDER OF THE TANK CONTENTS WOULD BE SWITCHED TO THE LP FLARE.     VENTING OF NITROGEN FROM THE TANK BEGAN ON JANUARY 15, 2022 AT APPROXIMATELY 0300 AND ENDED ON JANUARY 17, 2022 AT APPROXIMATELY 1000 HOURS WHEN FACILITY ENVIRONMENTAL PERSONNEL BECAME AWARE OF THE VENTING AND POTENTIAL FOR NATURAL GAS TO BE PRESENT IN THE VENT STREAM.  OPERATIONS WERE PROTECTIVELY CEASED PRIOR TO CONFIRMATION OF THE PRESENCE AND/OR QUANTITY OF ANY NATURAL GAS IN THE VENT.  LATER, IT WAS DETERMINED THAT NATURAL GAS MIXED WITH NITROGEN WAS IN FACT EMITTED.     THE PRIMARY ROOT CAUSE OF THE INCIDENT WAS THE EXCLUSION OF AN ENVIRONMENTAL SPECIALIST/ AIR PERMITTING SPECIALIST IN THE SIGN-OFF APPROVAL OF THE MOC. IF THAT INDIVIDUAL WAS INCLUDED IN THE MOC PROCESS, THE MOC WOULD HAVE NEVER BEEN EXECUTED SINCE THE LNG TANK IS NOT AN APPROVED EMISSION SOURCE.     TO PREVENT ANY RECURRENCE, ANY NITROGEN DISPLACEMENT ACTIVITY USING NATURAL GAS WILL EITHER DIRECT ANY VENT STREAM PURGED FROM THE LNG STORAGE TANKS TO A FLARE OR SUCH ACTIVITY WILL BE PERMITTED PURSUANT TO THE REGULATORY PERMIT IN LAC 33:III.309 OR OTHER APPROPRIATE AUTHORIZATION FROM THE LOUISIANA DEPARTMENT OF ENVIRONMENTAL QUALITY. IN ADDITION, THE FACILITY WILL ENSURE THAT ANY VENTING PROCEDURE AND ANY CHANGES THERETO ARE THOROUGHLY REVIEWED DURING THE MOC PROCESS AND ARE APPROVED BY APPROPRIATE AND RELEVANT STAFF, INCLUDING ENVIRONMENTAL STAFF, IN ADDITION TO OPERATIONS AND ENGINEERING STAFF. FINALLY, ANY PERSONNEL INVOLVED IN NITROGEN PURGING OPERATIONS FOR THE LNG STORAGE TANKS WILL RECEIVE ADDITIONAL TRAINING ON THE PROCEDURES AND REGULATORY REQUIREMENTS PRIOR TO ANY FUTURE NITROGEN DISPLACEMENT OPERATIONS.</t>
-  </si>
-  <si>
-    <t>ORIGINAL</t>
   </si>
   <si>
     <t>EVERSOURCE GAS COMPANY OF MASSACHUSETTS</t>
@@ -3580,7 +3577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEE5712-522A-4B59-B7CB-30FADB34326A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C543B04-DDE3-4E84-852F-FAF69C085C0B}">
   <sheetPr codeName="Sheet33"/>
   <dimension ref="A1:D224"/>
   <sheetViews>
@@ -6737,7 +6734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714D9FBB-CA80-4578-9D52-1DA6E566E805}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B877906E-D50D-45DF-A719-F541B5D10247}">
   <dimension ref="A1:HN33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -7467,7 +7464,7 @@
     </row>
     <row r="2" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>462</v>
@@ -7748,7 +7745,7 @@
     </row>
     <row r="3" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>462</v>
@@ -8008,7 +8005,7 @@
     </row>
     <row r="4" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>469</v>
@@ -8295,7 +8292,7 @@
     </row>
     <row r="5" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>462</v>
@@ -8573,7 +8570,7 @@
     </row>
     <row r="6" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>469</v>
@@ -8842,7 +8839,7 @@
     </row>
     <row r="7" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>462</v>
@@ -9114,7 +9111,7 @@
     </row>
     <row r="8" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>462</v>
@@ -9371,7 +9368,7 @@
     </row>
     <row r="9" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>462</v>
@@ -9643,7 +9640,7 @@
     </row>
     <row r="10" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>462</v>
@@ -9909,7 +9906,7 @@
     </row>
     <row r="11" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>469</v>
@@ -10169,7 +10166,7 @@
     </row>
     <row r="12" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>469</v>
@@ -10447,7 +10444,7 @@
     </row>
     <row r="13" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>462</v>
@@ -10722,7 +10719,7 @@
     </row>
     <row r="14" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>469</v>
@@ -11003,7 +11000,7 @@
     </row>
     <row r="15" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>462</v>
@@ -11266,7 +11263,7 @@
     </row>
     <row r="16" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>462</v>
@@ -11535,7 +11532,7 @@
     </row>
     <row r="17" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>462</v>
@@ -11807,7 +11804,7 @@
     </row>
     <row r="18" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>462</v>
@@ -12073,7 +12070,7 @@
     </row>
     <row r="19" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>469</v>
@@ -12342,7 +12339,7 @@
     </row>
     <row r="20" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>469</v>
@@ -12617,7 +12614,7 @@
     </row>
     <row r="21" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>462</v>
@@ -12883,7 +12880,7 @@
     </row>
     <row r="22" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>469</v>
@@ -13152,7 +13149,7 @@
     </row>
     <row r="23" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>469</v>
@@ -13448,7 +13445,7 @@
     </row>
     <row r="24" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>462</v>
@@ -13744,7 +13741,7 @@
     </row>
     <row r="25" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>462</v>
@@ -14028,7 +14025,7 @@
     </row>
     <row r="26" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>469</v>
@@ -14300,7 +14297,7 @@
     </row>
     <row r="27" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>462</v>
@@ -14587,7 +14584,7 @@
     </row>
     <row r="28" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>462</v>
@@ -14874,7 +14871,7 @@
     </row>
     <row r="29" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>462</v>
@@ -15155,7 +15152,7 @@
     </row>
     <row r="30" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>462</v>
@@ -15445,7 +15442,7 @@
     </row>
     <row r="31" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>462</v>
@@ -15723,7 +15720,7 @@
     </row>
     <row r="32" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>462</v>
@@ -16022,7 +16019,7 @@
     </row>
     <row r="33" spans="1:222" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="14">
-        <v>44712.391365740739</v>
+        <v>44742.398541666669</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>462</v>
@@ -16034,37 +16031,37 @@
         <v>20220003</v>
       </c>
       <c r="E33" s="12">
-        <v>36402</v>
+        <v>36711</v>
       </c>
       <c r="F33" s="14">
         <v>44620.350312499999</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>1019</v>
+        <v>934</v>
       </c>
       <c r="H33" s="12">
         <v>40195</v>
       </c>
       <c r="I33" s="12" t="s">
+        <v>1019</v>
+      </c>
+      <c r="J33" s="12" t="s">
         <v>1020</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="K33" s="12" t="s">
         <v>1021</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>1022</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>698</v>
       </c>
       <c r="M33" s="13" t="s">
+        <v>1022</v>
+      </c>
+      <c r="N33" s="15">
+        <v>44592.086805555555</v>
+      </c>
+      <c r="O33" s="12" t="s">
         <v>1023</v>
-      </c>
-      <c r="N33" s="15">
-        <v>44592.104166666664</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>1024</v>
       </c>
       <c r="P33" s="12" t="s">
         <v>469</v>
@@ -16139,7 +16136,7 @@
         <v>0</v>
       </c>
       <c r="BE33" s="12" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="BG33" s="12" t="s">
         <v>474</v>
@@ -16184,7 +16181,7 @@
         <v>478</v>
       </c>
       <c r="CN33" s="12" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="CO33" s="13" t="s">
         <v>480</v>
@@ -16196,7 +16193,7 @@
         <v>481</v>
       </c>
       <c r="CR33" s="13" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="CS33" s="13" t="s">
         <v>480</v>
@@ -16226,10 +16223,10 @@
         <v>481</v>
       </c>
       <c r="DC33" s="13" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="DD33" s="13" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="DE33" s="12" t="s">
         <v>469</v>
@@ -16250,56 +16247,61 @@
         <v>462</v>
       </c>
       <c r="DP33" s="12" t="s">
-        <v>707</v>
+        <v>485</v>
       </c>
       <c r="DQ33" s="12" t="s">
-        <v>708</v>
+        <v>486</v>
       </c>
       <c r="DR33" s="12" t="s">
-        <v>709</v>
+        <v>487</v>
       </c>
       <c r="DS33" s="12" t="s">
-        <v>708</v>
-      </c>
-      <c r="FH33" s="12" t="s">
-        <v>708</v>
-      </c>
-      <c r="FI33" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="EW33" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="EX33" s="12" t="s">
+        <v>1028</v>
+      </c>
+      <c r="EY33" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="EZ33" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="HD33" s="12" t="s">
         <v>1029</v>
       </c>
-      <c r="HD33" s="12" t="s">
+      <c r="HE33" s="12" t="s">
         <v>1030</v>
       </c>
-      <c r="HE33" s="12" t="s">
+      <c r="HF33" s="12" t="s">
         <v>1031</v>
       </c>
-      <c r="HF33" s="12" t="s">
+      <c r="HG33" s="13" t="s">
         <v>1032</v>
       </c>
-      <c r="HG33" s="13" t="s">
+      <c r="HI33" s="14">
+        <v>44713</v>
+      </c>
+      <c r="HJ33" s="12" t="s">
+        <v>1029</v>
+      </c>
+      <c r="HK33" s="12" t="s">
         <v>1033</v>
       </c>
-      <c r="HI33" s="14">
-        <v>44620</v>
-      </c>
-      <c r="HJ33" s="12" t="s">
-        <v>1030</v>
-      </c>
-      <c r="HK33" s="12" t="s">
+      <c r="HL33" s="13" t="s">
         <v>1034</v>
       </c>
-      <c r="HL33" s="13" t="s">
+      <c r="HM33" s="12" t="s">
+        <v>1031</v>
+      </c>
+      <c r="HN33" s="12" t="s">
         <v>1035</v>
-      </c>
-      <c r="HM33" s="12" t="s">
-        <v>1032</v>
-      </c>
-      <c r="HN33" s="12" t="s">
-        <v>1036</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>